<commit_message>
Modify requirements and excel naming
</commit_message>
<xml_diff>
--- a/mads_config.xlsx
+++ b/mads_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\Intern-IoT-Data-Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download_D_Drive\Github\Intern-IoT-Data-Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD5A28E-3C9C-40AE-A317-4400CA8E68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E716B5-A130-4E0B-8A7A-E05F48E8BB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26085" yWindow="1380" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="units_to_query" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -520,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>